<commit_message>
Cosas que se cambiaron con el profe
</commit_message>
<xml_diff>
--- a/Copia de ITF_ Mediciones durante experimento con ceros.xlsx
+++ b/Copia de ITF_ Mediciones durante experimento con ceros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Análisis datos Tempate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferce\Desktop\Cursos\Estadística-U\Tercero\Experimentos2\Proyecto final mediciones repetidas\proyecto_medidas_repetiras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4310188F-3DDF-44E0-941C-6ADD630FBD49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D64D70-A227-4A58-907F-3CFEA2AA1ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos" sheetId="14" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Cosecha" sheetId="12" r:id="rId11"/>
     <sheet name="Sobrevivencia" sheetId="15" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -495,7 +495,7 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -679,10 +679,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -7859,9 +7859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
@@ -10033,7 +10033,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -10171,11 +10171,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -10809,11 +10809,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -11448,11 +11448,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -12087,11 +12087,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -12730,7 +12730,7 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -13365,11 +13365,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -14008,7 +14008,7 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -14643,11 +14643,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>